<commit_message>
Problem 1 work, slight mod to prob 2
Alex and I worked on problem 1 last night and made some progress. I also
updated problem 2 with an estimate of the number of evaluations to reach
the desired error for the midpoint rule with 10 dimensions
</commit_message>
<xml_diff>
--- a/HW3/HW3_Prob2/HW3_Prob2_Error_comparison.xlsx
+++ b/HW3/HW3_Prob2/HW3_Prob2_Error_comparison.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\ME701\HW3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\ME701\HW3\HW3_Prob2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>FORTRAN MC</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>MP n = 10</t>
+  </si>
+  <si>
+    <t>Error &lt; 0.0001 would require ~ 1E19 evaluations</t>
   </si>
 </sst>
 </file>
@@ -789,11 +792,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="333602360"/>
-        <c:axId val="333602752"/>
+        <c:axId val="217594112"/>
+        <c:axId val="217594504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="333602360"/>
+        <c:axId val="217594112"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -903,12 +906,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333602752"/>
+        <c:crossAx val="217594504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="333602752"/>
+        <c:axId val="217594504"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1021,7 +1024,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333602360"/>
+        <c:crossAx val="217594112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1658,7 +1661,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1958,8 +1961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,6 +2548,9 @@
       <c r="D31" s="1">
         <v>1.06E-6</v>
       </c>
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>

</xml_diff>